<commit_message>
2021 post ops updates
</commit_message>
<xml_diff>
--- a/static/download/2021/RP3_APT_ASMA_2021_Jan_Dec.xlsx
+++ b/static/download/2021/RP3_APT_ASMA_2021_Jan_Dec.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="129">
   <si>
     <t>Data source</t>
   </si>
@@ -77,7 +77,7 @@
     <t>Belgium</t>
   </si>
   <si>
-    <t>Berlin/ Schoenefeld (EDDB)</t>
+    <t>Berlin Brandenburg (EDDB)</t>
   </si>
   <si>
     <t>EDDB</t>
@@ -393,6 +393,12 @@
   </si>
   <si>
     <t>UK airports removed</t>
+  </si>
+  <si>
+    <t>LFMN, LHBP</t>
+  </si>
+  <si>
+    <t>Airports updated with complete data set for 2021</t>
   </si>
 </sst>
 </file>
@@ -560,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -666,9 +672,6 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
@@ -712,14 +715,14 @@
       <selection activeCell="B7" sqref="B7" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.43"/>
-    <col customWidth="1" min="2" max="2" width="17.71"/>
-    <col customWidth="1" min="3" max="3" width="15.14"/>
-    <col customWidth="1" min="4" max="5" width="26.0"/>
-    <col customWidth="1" min="6" max="6" width="20.71"/>
-    <col customWidth="1" min="7" max="7" width="23.71"/>
+    <col customWidth="1" min="1" max="1" width="20.5"/>
+    <col customWidth="1" min="2" max="2" width="15.5"/>
+    <col customWidth="1" min="3" max="3" width="13.25"/>
+    <col customWidth="1" min="4" max="5" width="22.75"/>
+    <col customWidth="1" min="6" max="6" width="18.13"/>
+    <col customWidth="1" min="7" max="7" width="20.75"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -749,7 +752,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="9">
-        <v>44606.0</v>
+        <v>44665.0</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>5</v>
@@ -1390,14 +1393,14 @@
         <v>74</v>
       </c>
       <c r="D30" s="27">
-        <v>21289.0</v>
+        <v>26700.0</v>
       </c>
       <c r="E30" s="28">
         <f t="shared" si="2"/>
-        <v>0.4453003899</v>
+        <v>0.5411235955</v>
       </c>
       <c r="F30" s="27">
-        <v>9480.0</v>
+        <v>14448.0</v>
       </c>
       <c r="G30" s="28">
         <v>11.33</v>
@@ -1510,17 +1513,17 @@
         <v>90</v>
       </c>
       <c r="D35" s="27">
-        <v>9084.0</v>
+        <v>25446.0</v>
       </c>
       <c r="E35" s="28">
         <f t="shared" si="2"/>
-        <v>0.2874284456</v>
+        <v>0.6709109487</v>
       </c>
       <c r="F35" s="27">
-        <v>2611.0</v>
+        <v>17072.0</v>
       </c>
       <c r="G35" s="29">
-        <v>13.52</v>
+        <v>13.83</v>
       </c>
     </row>
     <row r="36" ht="12.75" customHeight="1">
@@ -1824,12 +1827,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.86"/>
-    <col customWidth="1" min="2" max="2" width="18.14"/>
-    <col customWidth="1" min="3" max="3" width="8.0"/>
-    <col customWidth="1" min="4" max="4" width="78.57"/>
+    <col customWidth="1" min="1" max="1" width="13.0"/>
+    <col customWidth="1" min="2" max="2" width="15.88"/>
+    <col customWidth="1" min="3" max="3" width="7.0"/>
+    <col customWidth="1" min="4" max="4" width="68.75"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -1859,22 +1862,30 @@
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="36"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="37"/>
+      <c r="A3" s="33">
+        <v>44665.0</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="37">
+        <v>2021.0</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="33"/>
-      <c r="B4" s="39"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="35"/>
-      <c r="D4" s="40"/>
+      <c r="D4" s="39"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="41"/>
-      <c r="B5" s="39"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="35"/>
-      <c r="D5" s="40"/>
+      <c r="D5" s="39"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>